<commit_message>
Feedback from sharon and rob
</commit_message>
<xml_diff>
--- a/reactive charts.xlsx
+++ b/reactive charts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luke.stephenson/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luke.stephenson/Documents/reactive-streams/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -197,19 +197,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.0</c:v>
@@ -254,19 +254,19 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -282,11 +282,11 @@
         </c:dLbls>
         <c:gapWidth val="50"/>
         <c:overlap val="100"/>
-        <c:axId val="-422063744"/>
-        <c:axId val="-422061424"/>
+        <c:axId val="-738473904"/>
+        <c:axId val="-738472128"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-422063744"/>
+        <c:axId val="-738473904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -331,7 +331,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-422061424"/>
+        <c:crossAx val="-738472128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -339,9 +339,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-422061424"/>
+        <c:axId val="-738472128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1.0"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="l"/>
@@ -373,7 +374,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-422063744"/>
+        <c:crossAx val="-738473904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -474,13 +475,27 @@
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr>
+            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
               <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="50" normalizeH="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
+                  <a:sysClr val="windowText" lastClr="000000">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  </a:sysClr>
                 </a:solidFill>
                 <a:latin typeface="+mj-lt"/>
                 <a:ea typeface="+mj-ea"/>
@@ -488,9 +503,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>TIMELINE</a:t>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" cap="all" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Timeline</a:t>
             </a:r>
+            <a:endParaRPr lang="en-US" b="0">
+              <a:effectLst/>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -507,13 +527,27 @@
         <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr>
+          <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
             <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="50" normalizeH="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:sysClr val="windowText" lastClr="000000">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
-                </a:schemeClr>
+                </a:sysClr>
               </a:solidFill>
               <a:latin typeface="+mj-lt"/>
               <a:ea typeface="+mj-ea"/>
@@ -529,7 +563,7 @@
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+        <c:grouping val="stacked"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
@@ -564,22 +598,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -618,22 +652,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -648,12 +682,12 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="80"/>
-        <c:overlap val="25"/>
-        <c:axId val="-397605440"/>
-        <c:axId val="-397603120"/>
+        <c:overlap val="100"/>
+        <c:axId val="-741651648"/>
+        <c:axId val="-741649328"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-397605440"/>
+        <c:axId val="-741651648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -695,7 +729,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-397603120"/>
+        <c:crossAx val="-741649328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -703,9 +737,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-397603120"/>
+        <c:axId val="-741649328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1.0"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="l"/>
@@ -726,7 +761,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-397605440"/>
+        <c:crossAx val="-741651648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1970,8 +2005,8 @@
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>800100</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
       <xdr:row>46</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
@@ -2260,8 +2295,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="R46" sqref="R46"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2297,19 +2332,19 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -2326,19 +2361,19 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -2375,22 +2410,22 @@
         <v>1</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E28">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F28">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G28">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H28">
         <v>1</v>
@@ -2401,22 +2436,22 @@
         <v>2</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F29">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G29">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H29">
         <v>1</v>

</xml_diff>